<commit_message>
filter primary location type is journal
</commit_message>
<xml_diff>
--- a/citations/publisher_emerald_2023_counts.xlsx
+++ b/citations/publisher_emerald_2023_counts.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B163"/>
+  <dimension ref="A1:B141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -382,37 +382,37 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Advances in education in diverse communities</t>
+          <t>Agricultural Finance Review</t>
         </is>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Advances in educational administration</t>
+          <t>Aircraft Engineering and Aerospace Technology</t>
         </is>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Advances in group processes</t>
+          <t>Anti-Corrosion Methods and Materials</t>
         </is>
       </c>
       <c r="B5">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Advances in health care management</t>
+          <t>Asia Pacific Journal of Marketing and Logistics</t>
         </is>
       </c>
       <c r="B6">
@@ -422,17 +422,17 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Advances in medical sociology</t>
+          <t>Asian Libraries</t>
         </is>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Advances in research ethics and integrity</t>
+          <t>Aslib Journal of Information Management</t>
         </is>
       </c>
       <c r="B8">
@@ -442,27 +442,27 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Advances in research on teaching</t>
+          <t>British Food Journal</t>
         </is>
       </c>
       <c r="B9">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Agricultural Finance Review</t>
+          <t>Career Development International</t>
         </is>
       </c>
       <c r="B10">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Aircraft Engineering and Aerospace Technology</t>
+          <t>China Agricultural Economic Review</t>
         </is>
       </c>
       <c r="B11">
@@ -472,17 +472,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Anti-Corrosion Methods and Materials</t>
+          <t>Corporate Communications An International Journal</t>
         </is>
       </c>
       <c r="B12">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Asia Pacific Journal of Marketing and Logistics</t>
+          <t>Corporate Governance</t>
         </is>
       </c>
       <c r="B13">
@@ -492,7 +492,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Asian Libraries</t>
+          <t>Digital Library Perspectives</t>
         </is>
       </c>
       <c r="B14">
@@ -502,17 +502,17 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Aslib Journal of Information Management</t>
+          <t>Disaster Prevention and Management An International Journal</t>
         </is>
       </c>
       <c r="B15">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>British Food Journal</t>
+          <t>Ecofeminism and Climate Change</t>
         </is>
       </c>
       <c r="B16">
@@ -522,27 +522,27 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Career Development International</t>
+          <t>Education + Training</t>
         </is>
       </c>
       <c r="B17">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>China Agricultural Economic Review</t>
+          <t>Electronic Resources Review</t>
         </is>
       </c>
       <c r="B18">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Community, environment and disaster risk management</t>
+          <t>Employee Relations</t>
         </is>
       </c>
       <c r="B19">
@@ -552,27 +552,27 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Corporate Communications An International Journal</t>
+          <t>Engineering Computations</t>
         </is>
       </c>
       <c r="B20">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Corporate Governance</t>
+          <t>Engineering Construction &amp; Architectural Management</t>
         </is>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Cutting-edge technologies in higher education</t>
+          <t>Environmental Management and Health</t>
         </is>
       </c>
       <c r="B22">
@@ -582,47 +582,47 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Digital Library Perspectives</t>
+          <t>Equality Diversity and Inclusion An International Journal</t>
         </is>
       </c>
       <c r="B23">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Disaster Prevention and Management An International Journal</t>
+          <t>European Business Review</t>
         </is>
       </c>
       <c r="B24">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Ecofeminism and Climate Change</t>
+          <t>European Journal of Innovation Management</t>
         </is>
       </c>
       <c r="B25">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Education + Training</t>
+          <t>European Journal of Marketing</t>
         </is>
       </c>
       <c r="B26">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Electronic Resources Review</t>
+          <t>Evidence-based HRM a Global Forum for Empirical Scholarship</t>
         </is>
       </c>
       <c r="B27">
@@ -632,7 +632,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Employee Relations</t>
+          <t>Facilities</t>
         </is>
       </c>
       <c r="B28">
@@ -642,197 +642,197 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Engineering Computations</t>
+          <t>Higher Education Skills and Work-based Learning</t>
         </is>
       </c>
       <c r="B29">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Engineering Construction &amp; Architectural Management</t>
+          <t>Industrial and Commercial Training</t>
         </is>
       </c>
       <c r="B30">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Environmental Management and Health</t>
+          <t>Industrial Management &amp; Data Systems</t>
         </is>
       </c>
       <c r="B31">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Equality Diversity and Inclusion An International Journal</t>
+          <t>Industrial Robot the international journal of robotics research and application</t>
         </is>
       </c>
       <c r="B32">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>European Business Review</t>
+          <t>International Journal of Architectural Research Archnet-IJAR</t>
         </is>
       </c>
       <c r="B33">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>European Journal of Innovation Management</t>
+          <t>International Journal of Bank Marketing</t>
         </is>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>8</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>European Journal of Marketing</t>
+          <t>International Journal of Climate Change Strategies and Management</t>
         </is>
       </c>
       <c r="B35">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Evidence-based HRM a Global Forum for Empirical Scholarship</t>
+          <t>International Journal of Contemporary Hospitality Management</t>
         </is>
       </c>
       <c r="B36">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>International Journal of Disaster Resilience in the Built Environment</t>
         </is>
       </c>
       <c r="B37">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Higher Education Skills and Work-based Learning</t>
+          <t>International Journal of Educational Management</t>
         </is>
       </c>
       <c r="B38">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Industrial and Commercial Training</t>
+          <t>International Journal of Emergency Services</t>
         </is>
       </c>
       <c r="B39">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Industrial Management &amp; Data Systems</t>
+          <t>International Journal of Emerging Markets</t>
         </is>
       </c>
       <c r="B40">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Industrial Robot the international journal of robotics research and application</t>
+          <t>International Journal of Entrepreneurial Behaviour &amp; Research</t>
         </is>
       </c>
       <c r="B41">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>International Journal of Architectural Research Archnet-IJAR</t>
+          <t>International Journal of Health Care Quality Assurance</t>
         </is>
       </c>
       <c r="B42">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>International Journal of Bank Marketing</t>
+          <t>International Journal of Health Governance</t>
         </is>
       </c>
       <c r="B43">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>International Journal of Climate Change Strategies and Management</t>
+          <t>International Journal of Information and Learning Technology</t>
         </is>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>International Journal of Contemporary Hospitality Management</t>
+          <t>International Journal of Managing Projects in Business</t>
         </is>
       </c>
       <c r="B45">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>International Journal of Disaster Resilience in the Built Environment</t>
+          <t>International Journal of Manpower</t>
         </is>
       </c>
       <c r="B46">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>International Journal of Educational Management</t>
+          <t>International Journal of Mentoring and Coaching in Education</t>
         </is>
       </c>
       <c r="B47">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>International Journal of Emergency Services</t>
+          <t>International Journal of Numerical Methods for Heat &amp;amp Fluid Flow</t>
         </is>
       </c>
       <c r="B48">
@@ -842,47 +842,47 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>International Journal of Emerging Markets</t>
+          <t>International Journal of Operations &amp; Production Management</t>
         </is>
       </c>
       <c r="B49">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>International Journal of Entrepreneurial Behaviour &amp; Research</t>
+          <t>International journal of organizational analysis</t>
         </is>
       </c>
       <c r="B50">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>International Journal of Health Care Quality Assurance</t>
+          <t>International Journal of Pharmaceutical and Healthcare Marketing</t>
         </is>
       </c>
       <c r="B51">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>International Journal of Health Governance</t>
+          <t>International Journal of Physical Distribution &amp; Logistics Management</t>
         </is>
       </c>
       <c r="B52">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>International Journal of Information and Learning Technology</t>
+          <t>International Journal of Prisoner Health</t>
         </is>
       </c>
       <c r="B53">
@@ -892,37 +892,37 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>International Journal of Managing Projects in Business</t>
+          <t>International Journal of Productivity and Performance Management</t>
         </is>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>International Journal of Manpower</t>
+          <t>International Journal of Quality &amp; Reliability Management</t>
         </is>
       </c>
       <c r="B55">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>International Journal of Mentoring and Coaching in Education</t>
+          <t>International Journal of Quality and Service Sciences</t>
         </is>
       </c>
       <c r="B56">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>International Journal of Numerical Methods for Heat &amp;amp Fluid Flow</t>
+          <t>International Journal of Service Industry Management</t>
         </is>
       </c>
       <c r="B57">
@@ -932,67 +932,67 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>International Journal of Operations &amp; Production Management</t>
+          <t>International Journal of Social Economics</t>
         </is>
       </c>
       <c r="B58">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>International journal of organizational analysis</t>
+          <t>International Journal of Sociology and Social Policy</t>
         </is>
       </c>
       <c r="B59">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>International Journal of Pharmaceutical and Healthcare Marketing</t>
+          <t>International Journal of Sustainability in Higher Education</t>
         </is>
       </c>
       <c r="B60">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>International Journal of Physical Distribution &amp; Logistics Management</t>
+          <t>International Journal of Workplace Health Management</t>
         </is>
       </c>
       <c r="B61">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>International Journal of Prisoner Health</t>
+          <t>Internet Research</t>
         </is>
       </c>
       <c r="B62">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>International Journal of Productivity and Performance Management</t>
+          <t>Journal for Multicultural Education</t>
         </is>
       </c>
       <c r="B63">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>International Journal of Quality &amp; Reliability Management</t>
+          <t>Journal of Aggression Conflict and Peace Research</t>
         </is>
       </c>
       <c r="B64">
@@ -1002,7 +1002,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>International Journal of Quality and Service Sciences</t>
+          <t>Journal of Asia Business Studies</t>
         </is>
       </c>
       <c r="B65">
@@ -1012,7 +1012,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>International Journal of Service Industry Management</t>
+          <t>Journal of Asian Business and Economic Studies</t>
         </is>
       </c>
       <c r="B66">
@@ -1022,7 +1022,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>International Journal of Social Economics</t>
+          <t>Journal of Business Strategy</t>
         </is>
       </c>
       <c r="B67">
@@ -1032,77 +1032,77 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>International Journal of Sociology and Social Policy</t>
+          <t>Journal of Chinese Economic and Foreign Trade Studies</t>
         </is>
       </c>
       <c r="B68">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>International Journal of Sustainability in Higher Education</t>
+          <t>Journal of Consumer Marketing</t>
         </is>
       </c>
       <c r="B69">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>International Journal of Workplace Health Management</t>
+          <t>Journal of Corporate Real Estate</t>
         </is>
       </c>
       <c r="B70">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Internet Research</t>
+          <t>Journal of Documentation</t>
         </is>
       </c>
       <c r="B71">
-        <v>4</v>
+        <v>12</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Journal for Multicultural Education</t>
+          <t>Journal of Educational Administration</t>
         </is>
       </c>
       <c r="B72">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Journal of Aggression Conflict and Peace Research</t>
+          <t>Journal of Engineering Design and Technology</t>
         </is>
       </c>
       <c r="B73">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Journal of Asia Business Studies</t>
+          <t>Journal of Enterprise Information Management</t>
         </is>
       </c>
       <c r="B74">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Journal of Asian Business and Economic Studies</t>
+          <t>Journal of Entrepreneurship and Public Policy</t>
         </is>
       </c>
       <c r="B75">
@@ -1112,37 +1112,37 @@
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Journal of Business Strategy</t>
+          <t>Journal of Facilities Management</t>
         </is>
       </c>
       <c r="B76">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Journal of Chinese Economic and Foreign Trade Studies</t>
+          <t>Journal of Financial Crime</t>
         </is>
       </c>
       <c r="B77">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Journal of Consumer Marketing</t>
+          <t>Journal of Financial Economic Policy</t>
         </is>
       </c>
       <c r="B78">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Journal of Corporate Real Estate</t>
+          <t>Journal of Historical Research in Marketing</t>
         </is>
       </c>
       <c r="B79">
@@ -1152,27 +1152,27 @@
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Journal of Documentation</t>
+          <t>Journal of Information Communication and Ethics in Society</t>
         </is>
       </c>
       <c r="B80">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Journal of Educational Administration</t>
+          <t>Journal of Intellectual Capital</t>
         </is>
       </c>
       <c r="B81">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Journal of Engineering Design and Technology</t>
+          <t>Journal of Investment Compliance</t>
         </is>
       </c>
       <c r="B82">
@@ -1182,37 +1182,37 @@
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Journal of Enterprise Information Management</t>
+          <t>Journal of Knowledge Management</t>
         </is>
       </c>
       <c r="B83">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Journal of Entrepreneurship and Public Policy</t>
+          <t>Journal of Management Development</t>
         </is>
       </c>
       <c r="B84">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Journal of Facilities Management</t>
+          <t>Journal of Managerial Psychology</t>
         </is>
       </c>
       <c r="B85">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Journal of Financial Crime</t>
+          <t>Journal of Manufacturing Technology Management</t>
         </is>
       </c>
       <c r="B86">
@@ -1222,7 +1222,7 @@
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Journal of Financial Economic Policy</t>
+          <t>Journal of Modelling in Management</t>
         </is>
       </c>
       <c r="B87">
@@ -1232,7 +1232,7 @@
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Journal of Historical Research in Marketing</t>
+          <t>Journal of Money Laundering Control</t>
         </is>
       </c>
       <c r="B88">
@@ -1242,7 +1242,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Journal of Information Communication and Ethics in Society</t>
+          <t>Journal of Organizational Ethnography</t>
         </is>
       </c>
       <c r="B89">
@@ -1252,7 +1252,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Journal of Intellectual Capital</t>
+          <t>Journal of Place Management and Development</t>
         </is>
       </c>
       <c r="B90">
@@ -1262,77 +1262,77 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Journal of Investment Compliance</t>
+          <t>Journal of Product &amp; Brand Management</t>
         </is>
       </c>
       <c r="B91">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Journal of Knowledge Management</t>
+          <t>Journal of Property Investment and Finance</t>
         </is>
       </c>
       <c r="B92">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Journal of Management Development</t>
+          <t>Journal of Public Procurement</t>
         </is>
       </c>
       <c r="B93">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Journal of Managerial Psychology</t>
+          <t>Journal of Quality in Maintenance Engineering</t>
         </is>
       </c>
       <c r="B94">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Journal of Manufacturing Technology Management</t>
+          <t>Journal of Research in Innovative Teaching &amp; Learning</t>
         </is>
       </c>
       <c r="B95">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Journal of Modelling in Management</t>
+          <t>Journal of service management</t>
         </is>
       </c>
       <c r="B96">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Journal of Money Laundering Control</t>
+          <t>Journal of Services Marketing</t>
         </is>
       </c>
       <c r="B97">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Journal of Organizational Ethnography</t>
+          <t>Journal of Small Business and Enterprise Development</t>
         </is>
       </c>
       <c r="B98">
@@ -1342,57 +1342,57 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Journal of Place Management and Development</t>
+          <t>Journal of Social Marketing</t>
         </is>
       </c>
       <c r="B99">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Journal of Product &amp; Brand Management</t>
+          <t>Journal of strategy and management</t>
         </is>
       </c>
       <c r="B100">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Journal of Property Investment and Finance</t>
+          <t>Journal of Tourism Futures</t>
         </is>
       </c>
       <c r="B101">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Journal of Public Procurement</t>
+          <t>Kybernetes</t>
         </is>
       </c>
       <c r="B102">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Journal of Quality in Maintenance Engineering</t>
+          <t>Leadership &amp; Organization Development Journal</t>
         </is>
       </c>
       <c r="B103">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Journal of Research in Innovative Teaching &amp; Learning</t>
+          <t>Leadership in health services</t>
         </is>
       </c>
       <c r="B104">
@@ -1402,27 +1402,27 @@
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Journal of service management</t>
+          <t>Management Decision</t>
         </is>
       </c>
       <c r="B105">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Journal of Services Marketing</t>
+          <t>Management of Environmental Quality An International Journal</t>
         </is>
       </c>
       <c r="B106">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Journal of Small Business and Enterprise Development</t>
+          <t>Management Research The Journal of the Iberoamerican Academy of Management</t>
         </is>
       </c>
       <c r="B107">
@@ -1432,57 +1432,57 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Journal of Social Marketing</t>
+          <t>Managerial Finance</t>
         </is>
       </c>
       <c r="B108">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Journal of strategy and management</t>
+          <t>Marketing Intelligence &amp; Planning</t>
         </is>
       </c>
       <c r="B109">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Journal of Tourism Futures</t>
+          <t>Measuring Business Excellence</t>
         </is>
       </c>
       <c r="B110">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Kybernetes</t>
+          <t>Meditari Accountancy Research</t>
         </is>
       </c>
       <c r="B111">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Leadership &amp; Organization Development Journal</t>
+          <t>Mental Health Review Journal</t>
         </is>
       </c>
       <c r="B112">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Leadership in health services</t>
+          <t>Modern Supply Chain Research and Applications</t>
         </is>
       </c>
       <c r="B113">
@@ -1492,7 +1492,7 @@
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Literacy research, practice and evaluation</t>
+          <t>Nutrition &amp; Food Science</t>
         </is>
       </c>
       <c r="B114">
@@ -1502,17 +1502,17 @@
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>Management Decision</t>
+          <t>On the Horizon The International Journal of Learning Futures</t>
         </is>
       </c>
       <c r="B115">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Management of Environmental Quality An International Journal</t>
+          <t>Online Information Review</t>
         </is>
       </c>
       <c r="B116">
@@ -1522,7 +1522,7 @@
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Management Research The Journal of the Iberoamerican Academy of Management</t>
+          <t>Open House International</t>
         </is>
       </c>
       <c r="B117">
@@ -1532,37 +1532,37 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Managerial Finance</t>
+          <t>Organization Management Journal</t>
         </is>
       </c>
       <c r="B118">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Marketing Intelligence &amp; Planning</t>
+          <t>Personnel Review</t>
         </is>
       </c>
       <c r="B119">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Measuring Business Excellence</t>
+          <t>Policing An International Journal</t>
         </is>
       </c>
       <c r="B120">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Meditari Accountancy Research</t>
+          <t>Program electronic library and information systems</t>
         </is>
       </c>
       <c r="B121">
@@ -1572,67 +1572,67 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Mental Health Review Journal</t>
+          <t>Qualitative Market Research An International Journal</t>
         </is>
       </c>
       <c r="B122">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Modern Supply Chain Research and Applications</t>
+          <t>Qualitative Research in Organizations and Management An International Journal</t>
         </is>
       </c>
       <c r="B123">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>New horizons in managerial and organizational cognition</t>
+          <t>Qualitative Research Journal</t>
         </is>
       </c>
       <c r="B124">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>Nutrition &amp; Food Science</t>
+          <t>Quality Assurance in Education</t>
         </is>
       </c>
       <c r="B125">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>On the Horizon The International Journal of Learning Futures</t>
+          <t>Rapid Prototyping Journal</t>
         </is>
       </c>
       <c r="B126">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
         <is>
-          <t>Online Information Review</t>
+          <t>Reference Reviews</t>
         </is>
       </c>
       <c r="B127">
-        <v>1</v>
+        <v>9</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>Open House International</t>
+          <t>Review of Accounting and Finance</t>
         </is>
       </c>
       <c r="B128">
@@ -1642,107 +1642,107 @@
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>Organization Management Journal</t>
+          <t>Review of Behavioral Finance</t>
         </is>
       </c>
       <c r="B129">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>Personnel Review</t>
+          <t>Smart and Sustainable Built Environment</t>
         </is>
       </c>
       <c r="B130">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>Policing An International Journal</t>
+          <t>Social Responsibility Journal</t>
         </is>
       </c>
       <c r="B131">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Program electronic library and information systems</t>
+          <t>Strategic HR Review</t>
         </is>
       </c>
       <c r="B132">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>Qualitative Market Research An International Journal</t>
+          <t>Supply Chain Management An International Journal</t>
         </is>
       </c>
       <c r="B133">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>Qualitative Research in Organizations and Management An International Journal</t>
+          <t>The Bottom Line Managing Library Finances</t>
         </is>
       </c>
       <c r="B134">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>Qualitative Research Journal</t>
+          <t>The International Journal of Logistics Management</t>
         </is>
       </c>
       <c r="B135">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
         <is>
-          <t>Quality Assurance in Education</t>
+          <t>The Journal of Risk Finance</t>
         </is>
       </c>
       <c r="B136">
-        <v>6</v>
+        <v>1</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>Rapid Prototyping Journal</t>
+          <t>The TQM Journal</t>
         </is>
       </c>
       <c r="B137">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>Reference Reviews</t>
+          <t>Transforming Government People Process and Policy</t>
         </is>
       </c>
       <c r="B138">
-        <v>9</v>
+        <v>1</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>Research in consumer behavior</t>
+          <t>Work Study</t>
         </is>
       </c>
       <c r="B139">
@@ -1752,240 +1752,20 @@
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>Research in economic history</t>
+          <t>World Journal of Science Technology and Sustainable Development</t>
         </is>
       </c>
       <c r="B140">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>Research in experimental economics</t>
+          <t>Young Consumers Insight and Ideas for Responsible Marketers</t>
         </is>
       </c>
       <c r="B141">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="142">
-      <c r="A142" t="inlineStr">
-        <is>
-          <t>Research in labor economics</t>
-        </is>
-      </c>
-      <c r="B142">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="143">
-      <c r="A143" t="inlineStr">
-        <is>
-          <t>Research in rural sociology and development</t>
-        </is>
-      </c>
-      <c r="B143">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="144">
-      <c r="A144" t="inlineStr">
-        <is>
-          <t>Research in social movements, conflicts and change</t>
-        </is>
-      </c>
-      <c r="B144">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="145">
-      <c r="A145" t="inlineStr">
-        <is>
-          <t>Research in the history of economic thought and methodology</t>
-        </is>
-      </c>
-      <c r="B145">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="146">
-      <c r="A146" t="inlineStr">
-        <is>
-          <t>Research in the sociology of organizations</t>
-        </is>
-      </c>
-      <c r="B146">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="147">
-      <c r="A147" t="inlineStr">
-        <is>
-          <t>Review of Accounting and Finance</t>
-        </is>
-      </c>
-      <c r="B147">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="148">
-      <c r="A148" t="inlineStr">
-        <is>
-          <t>Review of Behavioral Finance</t>
-        </is>
-      </c>
-      <c r="B148">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="149">
-      <c r="A149" t="inlineStr">
-        <is>
-          <t>Smart and Sustainable Built Environment</t>
-        </is>
-      </c>
-      <c r="B149">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="150">
-      <c r="A150" t="inlineStr">
-        <is>
-          <t>Social Responsibility Journal</t>
-        </is>
-      </c>
-      <c r="B150">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="151">
-      <c r="A151" t="inlineStr">
-        <is>
-          <t>Sociology of crime, law and deviance</t>
-        </is>
-      </c>
-      <c r="B151">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="152">
-      <c r="A152" t="inlineStr">
-        <is>
-          <t>Strategic HR Review</t>
-        </is>
-      </c>
-      <c r="B152">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="153">
-      <c r="A153" t="inlineStr">
-        <is>
-          <t>Studies in information</t>
-        </is>
-      </c>
-      <c r="B153">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="154">
-      <c r="A154" t="inlineStr">
-        <is>
-          <t>Supply Chain Management An International Journal</t>
-        </is>
-      </c>
-      <c r="B154">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="155">
-      <c r="A155" t="inlineStr">
-        <is>
-          <t>The Bottom Line Managing Library Finances</t>
-        </is>
-      </c>
-      <c r="B155">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="156">
-      <c r="A156" t="inlineStr">
-        <is>
-          <t>The International Journal of Logistics Management</t>
-        </is>
-      </c>
-      <c r="B156">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="157">
-      <c r="A157" t="inlineStr">
-        <is>
-          <t>The Journal of Risk Finance</t>
-        </is>
-      </c>
-      <c r="B157">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="158">
-      <c r="A158" t="inlineStr">
-        <is>
-          <t>The TQM Journal</t>
-        </is>
-      </c>
-      <c r="B158">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="159">
-      <c r="A159" t="inlineStr">
-        <is>
-          <t>Transforming Government People Process and Policy</t>
-        </is>
-      </c>
-      <c r="B159">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="160">
-      <c r="A160" t="inlineStr">
-        <is>
-          <t>Transport and sustainability</t>
-        </is>
-      </c>
-      <c r="B160">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="161">
-      <c r="A161" t="inlineStr">
-        <is>
-          <t>Work Study</t>
-        </is>
-      </c>
-      <c r="B161">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162">
-      <c r="A162" t="inlineStr">
-        <is>
-          <t>World Journal of Science Technology and Sustainable Development</t>
-        </is>
-      </c>
-      <c r="B162">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="163">
-      <c r="A163" t="inlineStr">
-        <is>
-          <t>Young Consumers Insight and Ideas for Responsible Marketers</t>
-        </is>
-      </c>
-      <c r="B163">
         <v>3</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updating type journal and non-journal
</commit_message>
<xml_diff>
--- a/citations/publisher_emerald_2023_counts.xlsx
+++ b/citations/publisher_emerald_2023_counts.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B141"/>
+  <dimension ref="A1:B124"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -372,37 +372,37 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Accounting Auditing &amp; Accountability Journal</t>
+          <t>Academia Revista Latinoamericana de Administración</t>
         </is>
       </c>
       <c r="B2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Agricultural Finance Review</t>
+          <t>Accounting Auditing &amp; Accountability Journal</t>
         </is>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Aircraft Engineering and Aerospace Technology</t>
+          <t>African Journal of Economic and Management Studies</t>
         </is>
       </c>
       <c r="B4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Anti-Corrosion Methods and Materials</t>
+          <t>American Journal of Business</t>
         </is>
       </c>
       <c r="B5">
@@ -416,13 +416,13 @@
         </is>
       </c>
       <c r="B6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Asian Libraries</t>
+          <t>Aslib Journal of Information Management</t>
         </is>
       </c>
       <c r="B7">
@@ -432,11 +432,11 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Aslib Journal of Information Management</t>
+          <t>Aslib Proceedings</t>
         </is>
       </c>
       <c r="B8">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -446,7 +446,7 @@
         </is>
       </c>
       <c r="B9">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -456,23 +456,23 @@
         </is>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>China Agricultural Economic Review</t>
+          <t>Corporate Governance</t>
         </is>
       </c>
       <c r="B11">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Corporate Communications An International Journal</t>
+          <t>Cross Cultural &amp; Strategic Management</t>
         </is>
       </c>
       <c r="B12">
@@ -482,7 +482,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Corporate Governance</t>
+          <t>Data Technologies and Applications</t>
         </is>
       </c>
       <c r="B13">
@@ -506,7 +506,7 @@
         </is>
       </c>
       <c r="B15">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16">
@@ -516,7 +516,7 @@
         </is>
       </c>
       <c r="B16">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -526,63 +526,63 @@
         </is>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Electronic Resources Review</t>
+          <t>Engineering Computations</t>
         </is>
       </c>
       <c r="B18">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Employee Relations</t>
+          <t>Engineering Construction &amp; Architectural Management</t>
         </is>
       </c>
       <c r="B19">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Engineering Computations</t>
+          <t>English Teaching Practice &amp; Critique</t>
         </is>
       </c>
       <c r="B20">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Engineering Construction &amp; Architectural Management</t>
+          <t>Environmental Management and Health</t>
         </is>
       </c>
       <c r="B21">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Environmental Management and Health</t>
+          <t>European Journal of Marketing</t>
         </is>
       </c>
       <c r="B22">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Equality Diversity and Inclusion An International Journal</t>
+          <t>Gender in Management An International Journal</t>
         </is>
       </c>
       <c r="B23">
@@ -592,17 +592,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>European Business Review</t>
+          <t>Higher Education Skills and Work-based Learning</t>
         </is>
       </c>
       <c r="B24">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>European Journal of Innovation Management</t>
+          <t>Human Resource Management International Digest</t>
         </is>
       </c>
       <c r="B25">
@@ -612,27 +612,27 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>European Journal of Marketing</t>
+          <t>Industrial Management &amp; Data Systems</t>
         </is>
       </c>
       <c r="B26">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Evidence-based HRM a Global Forum for Empirical Scholarship</t>
+          <t>Industrial Robot the international journal of robotics research and application</t>
         </is>
       </c>
       <c r="B27">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Facilities</t>
+          <t>Information and Learning Sciences</t>
         </is>
       </c>
       <c r="B28">
@@ -642,47 +642,47 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Higher Education Skills and Work-based Learning</t>
+          <t>Information Management &amp; Computer Security</t>
         </is>
       </c>
       <c r="B29">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Industrial and Commercial Training</t>
+          <t>Innovation &amp; Management Review</t>
         </is>
       </c>
       <c r="B30">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Industrial Management &amp; Data Systems</t>
+          <t>International Journal of Bank Marketing</t>
         </is>
       </c>
       <c r="B31">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Industrial Robot the international journal of robotics research and application</t>
+          <t>International Journal of Climate Change Strategies and Management</t>
         </is>
       </c>
       <c r="B32">
-        <v>1</v>
+        <v>6</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>International Journal of Architectural Research Archnet-IJAR</t>
+          <t>International Journal of Conflict Management</t>
         </is>
       </c>
       <c r="B33">
@@ -692,57 +692,57 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>International Journal of Bank Marketing</t>
+          <t>International Journal of Contemporary Hospitality Management</t>
         </is>
       </c>
       <c r="B34">
-        <v>8</v>
+        <v>3</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>International Journal of Climate Change Strategies and Management</t>
+          <t>International Journal of Development Issues</t>
         </is>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>International Journal of Contemporary Hospitality Management</t>
+          <t>International Journal of Disaster Resilience in the Built Environment</t>
         </is>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>International Journal of Disaster Resilience in the Built Environment</t>
+          <t>International Journal of Educational Management</t>
         </is>
       </c>
       <c r="B37">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>International Journal of Educational Management</t>
+          <t>International Journal of Entrepreneurial Behaviour &amp; Research</t>
         </is>
       </c>
       <c r="B38">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>International Journal of Emergency Services</t>
+          <t>International Journal of Manpower</t>
         </is>
       </c>
       <c r="B39">
@@ -752,37 +752,37 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>International Journal of Emerging Markets</t>
+          <t>International Journal of Migration Health and Social Care</t>
         </is>
       </c>
       <c r="B40">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>International Journal of Entrepreneurial Behaviour &amp; Research</t>
+          <t>International Journal of Operations &amp; Production Management</t>
         </is>
       </c>
       <c r="B41">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>International Journal of Health Care Quality Assurance</t>
+          <t>International Journal of Pharmaceutical and Healthcare Marketing</t>
         </is>
       </c>
       <c r="B42">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>International Journal of Health Governance</t>
+          <t>International Journal of Physical Distribution &amp; Logistics Management</t>
         </is>
       </c>
       <c r="B43">
@@ -792,17 +792,17 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>International Journal of Information and Learning Technology</t>
+          <t>International Journal of Public Sector Management</t>
         </is>
       </c>
       <c r="B44">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>International Journal of Managing Projects in Business</t>
+          <t>International Journal of Quality &amp; Reliability Management</t>
         </is>
       </c>
       <c r="B45">
@@ -812,7 +812,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>International Journal of Manpower</t>
+          <t>International Journal of Retail &amp; Distribution Management</t>
         </is>
       </c>
       <c r="B46">
@@ -822,7 +822,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>International Journal of Mentoring and Coaching in Education</t>
+          <t>International Journal of Sociology and Social Policy</t>
         </is>
       </c>
       <c r="B47">
@@ -832,37 +832,37 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>International Journal of Numerical Methods for Heat &amp;amp Fluid Flow</t>
+          <t>International Journal of Sports Marketing and Sponsorship</t>
         </is>
       </c>
       <c r="B48">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>International Journal of Operations &amp; Production Management</t>
+          <t>International Journal of Sustainability in Higher Education</t>
         </is>
       </c>
       <c r="B49">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>International journal of organizational analysis</t>
+          <t>International Journal of Workplace Health Management</t>
         </is>
       </c>
       <c r="B50">
-        <v>1</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>International Journal of Pharmaceutical and Healthcare Marketing</t>
+          <t>International Marketing Review</t>
         </is>
       </c>
       <c r="B51">
@@ -872,17 +872,17 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>International Journal of Physical Distribution &amp; Logistics Management</t>
+          <t>Internet Research</t>
         </is>
       </c>
       <c r="B52">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>International Journal of Prisoner Health</t>
+          <t>Journal for Multicultural Education</t>
         </is>
       </c>
       <c r="B53">
@@ -892,17 +892,17 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>International Journal of Productivity and Performance Management</t>
+          <t>Journal of Accounting &amp; Organizational Change</t>
         </is>
       </c>
       <c r="B54">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>International Journal of Quality &amp; Reliability Management</t>
+          <t>Journal of Aggression Conflict and Peace Research</t>
         </is>
       </c>
       <c r="B55">
@@ -912,17 +912,17 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>International Journal of Quality and Service Sciences</t>
+          <t>Journal of Business Strategy</t>
         </is>
       </c>
       <c r="B56">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>International Journal of Service Industry Management</t>
+          <t>Journal of Chinese Economic and Foreign Trade Studies</t>
         </is>
       </c>
       <c r="B57">
@@ -932,7 +932,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>International Journal of Social Economics</t>
+          <t>Journal of Communication Management</t>
         </is>
       </c>
       <c r="B58">
@@ -942,17 +942,17 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>International Journal of Sociology and Social Policy</t>
+          <t>Journal of Consumer Marketing</t>
         </is>
       </c>
       <c r="B59">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>International Journal of Sustainability in Higher Education</t>
+          <t>Journal of Documentation</t>
         </is>
       </c>
       <c r="B60">
@@ -962,37 +962,37 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>International Journal of Workplace Health Management</t>
+          <t>Journal of Educational Administration</t>
         </is>
       </c>
       <c r="B61">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>Internet Research</t>
+          <t>Journal of Engineering Design and Technology</t>
         </is>
       </c>
       <c r="B62">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>Journal for Multicultural Education</t>
+          <t>Journal of Enterprising Communities People and Places in the Global Economy</t>
         </is>
       </c>
       <c r="B63">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>Journal of Aggression Conflict and Peace Research</t>
+          <t>Journal of Entrepreneurship and Public Policy</t>
         </is>
       </c>
       <c r="B64">
@@ -1002,27 +1002,27 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>Journal of Asia Business Studies</t>
+          <t>Journal of Entrepreneurship in Emerging Economies</t>
         </is>
       </c>
       <c r="B65">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>Journal of Asian Business and Economic Studies</t>
+          <t>Journal of Facilities Management</t>
         </is>
       </c>
       <c r="B66">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>Journal of Business Strategy</t>
+          <t>Journal of Fashion Marketing and Management</t>
         </is>
       </c>
       <c r="B67">
@@ -1032,7 +1032,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>Journal of Chinese Economic and Foreign Trade Studies</t>
+          <t>Journal of Global Responsibility</t>
         </is>
       </c>
       <c r="B68">
@@ -1042,47 +1042,47 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>Journal of Consumer Marketing</t>
+          <t>Journal of Health Organization and Management</t>
         </is>
       </c>
       <c r="B69">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>Journal of Corporate Real Estate</t>
+          <t>Journal of Historical Research in Marketing</t>
         </is>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>Journal of Documentation</t>
+          <t>Journal of Hospitality and Tourism Insights</t>
         </is>
       </c>
       <c r="B71">
-        <v>12</v>
+        <v>1</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>Journal of Educational Administration</t>
+          <t>Journal of Intellectual Capital</t>
         </is>
       </c>
       <c r="B72">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>Journal of Engineering Design and Technology</t>
+          <t>Journal of International Education in Business</t>
         </is>
       </c>
       <c r="B73">
@@ -1092,77 +1092,77 @@
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>Journal of Enterprise Information Management</t>
+          <t>Journal of International Trade Law and Policy</t>
         </is>
       </c>
       <c r="B74">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>Journal of Entrepreneurship and Public Policy</t>
+          <t>Journal of Knowledge Management</t>
         </is>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>Journal of Facilities Management</t>
+          <t>Journal of Management Development</t>
         </is>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>Journal of Financial Crime</t>
+          <t>Journal of Managerial Psychology</t>
         </is>
       </c>
       <c r="B77">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>Journal of Financial Economic Policy</t>
+          <t>Journal of Organizational Change Management</t>
         </is>
       </c>
       <c r="B78">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>Journal of Historical Research in Marketing</t>
+          <t>Journal of Product &amp; Brand Management</t>
         </is>
       </c>
       <c r="B79">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>Journal of Information Communication and Ethics in Society</t>
+          <t>Journal of Public Mental Health</t>
         </is>
       </c>
       <c r="B80">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>Journal of Intellectual Capital</t>
+          <t>Journal of service management</t>
         </is>
       </c>
       <c r="B81">
@@ -1172,17 +1172,17 @@
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>Journal of Investment Compliance</t>
+          <t>Journal of Services Marketing</t>
         </is>
       </c>
       <c r="B82">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>Journal of Knowledge Management</t>
+          <t>Journal of Small Business and Enterprise Development</t>
         </is>
       </c>
       <c r="B83">
@@ -1192,47 +1192,47 @@
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>Journal of Management Development</t>
+          <t>Journal of strategy and management</t>
         </is>
       </c>
       <c r="B84">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>Journal of Managerial Psychology</t>
+          <t>Journal of Tourism Futures</t>
         </is>
       </c>
       <c r="B85">
-        <v>8</v>
+        <v>1</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>Journal of Manufacturing Technology Management</t>
+          <t>Journal of Workplace Learning</t>
         </is>
       </c>
       <c r="B86">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>Journal of Modelling in Management</t>
+          <t>Kybernetes</t>
         </is>
       </c>
       <c r="B87">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>Journal of Money Laundering Control</t>
+          <t>Library Hi Tech</t>
         </is>
       </c>
       <c r="B88">
@@ -1242,7 +1242,7 @@
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>Journal of Organizational Ethnography</t>
+          <t>Library Hi Tech News</t>
         </is>
       </c>
       <c r="B89">
@@ -1252,7 +1252,7 @@
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>Journal of Place Management and Development</t>
+          <t>Library Management</t>
         </is>
       </c>
       <c r="B90">
@@ -1262,27 +1262,27 @@
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>Journal of Product &amp; Brand Management</t>
+          <t>Library Review</t>
         </is>
       </c>
       <c r="B91">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>Journal of Property Investment and Finance</t>
+          <t>Management Decision</t>
         </is>
       </c>
       <c r="B92">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>Journal of Public Procurement</t>
+          <t>Management Research Review</t>
         </is>
       </c>
       <c r="B93">
@@ -1292,7 +1292,7 @@
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>Journal of Quality in Maintenance Engineering</t>
+          <t>Managerial Finance</t>
         </is>
       </c>
       <c r="B94">
@@ -1302,7 +1302,7 @@
     <row r="95">
       <c r="A95" t="inlineStr">
         <is>
-          <t>Journal of Research in Innovative Teaching &amp; Learning</t>
+          <t>Managing Service Quality</t>
         </is>
       </c>
       <c r="B95">
@@ -1312,27 +1312,27 @@
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>Journal of service management</t>
+          <t>OCLC Systems &amp; Services</t>
         </is>
       </c>
       <c r="B96">
-        <v>7</v>
+        <v>1</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>Journal of Services Marketing</t>
+          <t>On the Horizon The International Journal of Learning Futures</t>
         </is>
       </c>
       <c r="B97">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>Journal of Small Business and Enterprise Development</t>
+          <t>Online Information Review</t>
         </is>
       </c>
       <c r="B98">
@@ -1342,77 +1342,77 @@
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>Journal of Social Marketing</t>
+          <t>Organization Management Journal</t>
         </is>
       </c>
       <c r="B99">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>Journal of strategy and management</t>
+          <t>Performance Measurement and Metrics</t>
         </is>
       </c>
       <c r="B100">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>Journal of Tourism Futures</t>
+          <t>Personnel Review</t>
         </is>
       </c>
       <c r="B101">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Kybernetes</t>
+          <t>Policing An International Journal</t>
         </is>
       </c>
       <c r="B102">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>Leadership &amp; Organization Development Journal</t>
+          <t>Qualitative Market Research An International Journal</t>
         </is>
       </c>
       <c r="B103">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
         <is>
-          <t>Leadership in health services</t>
+          <t>Qualitative Research in Accounting &amp; Management</t>
         </is>
       </c>
       <c r="B104">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
         <is>
-          <t>Management Decision</t>
+          <t>Qualitative Research in Organizations and Management An International Journal</t>
         </is>
       </c>
       <c r="B105">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
         <is>
-          <t>Management of Environmental Quality An International Journal</t>
+          <t>Qualitative Research Journal</t>
         </is>
       </c>
       <c r="B106">
@@ -1422,7 +1422,7 @@
     <row r="107">
       <c r="A107" t="inlineStr">
         <is>
-          <t>Management Research The Journal of the Iberoamerican Academy of Management</t>
+          <t>Quality in Ageing and Older Adults</t>
         </is>
       </c>
       <c r="B107">
@@ -1432,47 +1432,47 @@
     <row r="108">
       <c r="A108" t="inlineStr">
         <is>
-          <t>Managerial Finance</t>
+          <t>Rapid Prototyping Journal</t>
         </is>
       </c>
       <c r="B108">
-        <v>3</v>
+        <v>9</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
         <is>
-          <t>Marketing Intelligence &amp; Planning</t>
+          <t>Records Management Journal</t>
         </is>
       </c>
       <c r="B109">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
         <is>
-          <t>Measuring Business Excellence</t>
+          <t>Reference Reviews</t>
         </is>
       </c>
       <c r="B110">
-        <v>1</v>
+        <v>10</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
         <is>
-          <t>Meditari Accountancy Research</t>
+          <t>Reference Services Review</t>
         </is>
       </c>
       <c r="B111">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
         <is>
-          <t>Mental Health Review Journal</t>
+          <t>Review of Economics and Political Science</t>
         </is>
       </c>
       <c r="B112">
@@ -1482,27 +1482,27 @@
     <row r="113">
       <c r="A113" t="inlineStr">
         <is>
-          <t>Modern Supply Chain Research and Applications</t>
+          <t>Review of International Business and Strategy</t>
         </is>
       </c>
       <c r="B113">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
         <is>
-          <t>Nutrition &amp; Food Science</t>
+          <t>Sensor Review</t>
         </is>
       </c>
       <c r="B114">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
         <is>
-          <t>On the Horizon The International Journal of Learning Futures</t>
+          <t>Strategic HR Review</t>
         </is>
       </c>
       <c r="B115">
@@ -1512,27 +1512,27 @@
     <row r="116">
       <c r="A116" t="inlineStr">
         <is>
-          <t>Online Information Review</t>
+          <t>Studies in Graduate and Postdoctoral Education</t>
         </is>
       </c>
       <c r="B116">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
         <is>
-          <t>Open House International</t>
+          <t>Supply Chain Management An International Journal</t>
         </is>
       </c>
       <c r="B117">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>Organization Management Journal</t>
+          <t>The Electronic Library</t>
         </is>
       </c>
       <c r="B118">
@@ -1542,27 +1542,27 @@
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>Personnel Review</t>
+          <t>The Journal of Risk Finance</t>
         </is>
       </c>
       <c r="B119">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
         <is>
-          <t>Policing An International Journal</t>
+          <t>The Learning Organization</t>
         </is>
       </c>
       <c r="B120">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
         <is>
-          <t>Program electronic library and information systems</t>
+          <t>Transforming Government People Process and Policy</t>
         </is>
       </c>
       <c r="B121">
@@ -1572,17 +1572,17 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>Qualitative Market Research An International Journal</t>
+          <t>Vilakshan – XIMB Journal of Management</t>
         </is>
       </c>
       <c r="B122">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
         <is>
-          <t>Qualitative Research in Organizations and Management An International Journal</t>
+          <t>Work Study</t>
         </is>
       </c>
       <c r="B123">
@@ -1592,180 +1592,10 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>Qualitative Research Journal</t>
+          <t>Young Consumers Insight and Ideas for Responsible Marketers</t>
         </is>
       </c>
       <c r="B124">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="125">
-      <c r="A125" t="inlineStr">
-        <is>
-          <t>Quality Assurance in Education</t>
-        </is>
-      </c>
-      <c r="B125">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="126">
-      <c r="A126" t="inlineStr">
-        <is>
-          <t>Rapid Prototyping Journal</t>
-        </is>
-      </c>
-      <c r="B126">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="127">
-      <c r="A127" t="inlineStr">
-        <is>
-          <t>Reference Reviews</t>
-        </is>
-      </c>
-      <c r="B127">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" t="inlineStr">
-        <is>
-          <t>Review of Accounting and Finance</t>
-        </is>
-      </c>
-      <c r="B128">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="129">
-      <c r="A129" t="inlineStr">
-        <is>
-          <t>Review of Behavioral Finance</t>
-        </is>
-      </c>
-      <c r="B129">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="130">
-      <c r="A130" t="inlineStr">
-        <is>
-          <t>Smart and Sustainable Built Environment</t>
-        </is>
-      </c>
-      <c r="B130">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="131">
-      <c r="A131" t="inlineStr">
-        <is>
-          <t>Social Responsibility Journal</t>
-        </is>
-      </c>
-      <c r="B131">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="132">
-      <c r="A132" t="inlineStr">
-        <is>
-          <t>Strategic HR Review</t>
-        </is>
-      </c>
-      <c r="B132">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133">
-      <c r="A133" t="inlineStr">
-        <is>
-          <t>Supply Chain Management An International Journal</t>
-        </is>
-      </c>
-      <c r="B133">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="134">
-      <c r="A134" t="inlineStr">
-        <is>
-          <t>The Bottom Line Managing Library Finances</t>
-        </is>
-      </c>
-      <c r="B134">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="135">
-      <c r="A135" t="inlineStr">
-        <is>
-          <t>The International Journal of Logistics Management</t>
-        </is>
-      </c>
-      <c r="B135">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136">
-      <c r="A136" t="inlineStr">
-        <is>
-          <t>The Journal of Risk Finance</t>
-        </is>
-      </c>
-      <c r="B136">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="137">
-      <c r="A137" t="inlineStr">
-        <is>
-          <t>The TQM Journal</t>
-        </is>
-      </c>
-      <c r="B137">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="138">
-      <c r="A138" t="inlineStr">
-        <is>
-          <t>Transforming Government People Process and Policy</t>
-        </is>
-      </c>
-      <c r="B138">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="139">
-      <c r="A139" t="inlineStr">
-        <is>
-          <t>Work Study</t>
-        </is>
-      </c>
-      <c r="B139">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="140">
-      <c r="A140" t="inlineStr">
-        <is>
-          <t>World Journal of Science Technology and Sustainable Development</t>
-        </is>
-      </c>
-      <c r="B140">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="141">
-      <c r="A141" t="inlineStr">
-        <is>
-          <t>Young Consumers Insight and Ideas for Responsible Marketers</t>
-        </is>
-      </c>
-      <c r="B141">
         <v>3</v>
       </c>
     </row>

</xml_diff>